<commit_message>
update mcmc after errors
</commit_message>
<xml_diff>
--- a/lit_search/table_studies.xlsx
+++ b/lit_search/table_studies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\g01-metaanalysis\lit_search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5D2693-0078-4A50-81C1-C8155ADAC15F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2743E2BD-4E76-491B-B15F-A909B442B05A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D097B5BB-D942-4261-9253-69DA95D5109F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="289">
   <si>
     <t>Citation</t>
   </si>
@@ -884,7 +884,22 @@
     <t>io</t>
   </si>
   <si>
-    <t>Diatraea grandiosella</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Diatraea</t>
+  </si>
+  <si>
+    <t>grandiosella</t>
   </si>
 </sst>
 </file>
@@ -1265,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE733E50-313F-4145-BB46-E9C671DF6AD9}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,6 +1296,18 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E1" t="s">
+        <v>286</v>
+      </c>
       <c r="F1" s="3" t="s">
         <v>162</v>
       </c>
@@ -3667,7 +3694,10 @@
         <v>187</v>
       </c>
       <c r="K64" t="s">
-        <v>283</v>
+        <v>287</v>
+      </c>
+      <c r="L64" t="s">
+        <v>288</v>
       </c>
       <c r="M64" t="s">
         <v>179</v>

</xml_diff>